<commit_message>
Fix overview_and_products_services.csv and other changes
</commit_message>
<xml_diff>
--- a/phase_1/data/overview_and_products_services.xlsx
+++ b/phase_1/data/overview_and_products_services.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,59 +436,645 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Overview</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Products &amp; Services</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Zoominfo Revenue</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>RocketReach Revenue</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>General Revenue</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Founder/CEO</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Employee</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Year Founded</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Business Type</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> I'm sorry, but as an AI language model, I cannot provide a specific response without the full text of your query. Can you please give me more context or details about what you need help with?
-</t>
+          <t>Veritas Capital Fund Management LLC</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> I'm sorry, but the information you provided does not include any specific details about the products and services of Yamada. Can you please provide more context or information so that I can better understand what you are referring to?
-</t>
-        </is>
-      </c>
+          <t xml:space="preserve"> Veritas Capital is a technology-focused private equity firm based in New York, with over $40 billion in assets under management. The company primarily invests in technology or technology-enabled solutions, particularly those operating at the intersection of technology and government. Veritas Capital's team includes Managing Director Rushin Shah, who previously founded Nine27 Capital Management, and Hardik Patel. The firm guides portfolio companies' strategies as board members.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veritas Capital Fund Management LLC is a New York-based private equity firm, founded in 1992, with a focus on investing in companies that provide critical products and services, primarily technology-enabled solutions, to both government and commercial customers worldwide. The firm has over $40 billion in assets under management and is known for its longstanding investment in technology companies operating at the intersection of technology and government.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> I apologize for the inconvenience, but as an AI language model, I do not have access to external resources such as the internet or a navigation system. However, according to my research on Yamada, it is a Japanese company that manufactures and sells various electronic devices, including smartphones, laptops, and televisions. The company was founded in 1967 and has since established itself as one of the leading electronics manufacturers in Japan.
-In recent years, Yamada has expanded its business globally and opened up branches in many countries. The company's products are known for their high quality, reliability, and innovation. In addition to manufacturing electronic devices, Yamada also provides maintenance services, such as repair and replacement parts, for its customers.
-It is important to note that while the bing search engine may not always provide accurate or complete information, it can still be a helpful tool in discovering new companies and products. However, when using online resources, it is crucial to verify the credibility of the information and check multiple sources to ensure accuracy.
-Based on the information you have from your conversation, consider three Yamada product lines: smartphones, laptops, and televisions. 
-Each line has a certain quality score ranging between 1-10 (1 being the lowest and 10 being the highest), reliability score from 1-5 (1 being very unreliable and 5 being extremely reliable), and innovation score from 1-3 (1 is least innovative and 3 is most innovative). 
-We know that:
-1. The smartphone quality score is higher than the laptop and television quality scores combined.
-2. The reliability score for smartphones is exactly in the middle of the laptop and television reliability scores.
-3. The innovation score for televisions is higher than the laptops but lower than the smartphones.
-Question: What are the quality, reliability, and innovation scores for each product line?
-First let's use deductive logic to analyze the first clue: The smartphone quality score is higher than the laptop and television quality scores combined. This means that the smartphone must have a score of 8 or 9 while laptops and televisions combined cannot be more than 7. 
-Now, consider the second clue: The reliability score for smartphones is exactly in the middle of the laptop and television reliability scores. Since the reliability scores are 1-5, this would mean that the reliability score for smartphones must be 3 (the middle number). This means laptops and televisions combined cannot have a score of 2 or 4.
-The last clue gives us: The innovation score for televisions is higher than the laptops but lower than the smartphones. The numbers in the 1-3 range are already used by the quality and reliability scores, so this leaves 2 as the only possibility for the innovation score of the television. This means that the laptops must have a score of 5 (since it's the highest number that can be assigned).
-Finally, we use inductive logic to assign the remaining values: Since the smartphones have an 8 or 9 quality score and an 3 reliability score, this leaves 1-6 for the innovation score. The only scores left are 2, 4, 6, 7, and 8. But the television has a 2 for its innovation score. Therefore, it makes sense that the smartphone has to have a higher innovation score of either 5 or 7. Since the televisions must be lower than the smartphones in terms of innovation, the remaining scores for smartphones (1-7) will have to match with their respective quality and reliability scores which leave 1-3 for the televisions.
-Answer: 
-Smartphones - Quality Score 8/9, Reliability Score 3, Innovation Score 6/7
-Laptops - Quality Score 7/8, Reliability Score 5, Innovation Score 4
-Televisions - Quality Score 6/7, Reliability Score 2, Innovation Score 1/3
+          <t>Bluestone Equity Partners</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Founded by Bobby Sharma, a Duke Law graduate with deep industry connections on over 500+ LinkedIn profiles and Harvard Business School education from Jake Harris's profile details for Bluestone Equity Partners; they specialize in strategic capital partnerships within Sports, Media &amp; Entertainment sectors.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Situated at the prestigious Chrysler Building in New York, Bluestone Equity Partners stands as an institutionally-backed private equity firm that invests primarily within outsourcing services and environmental sectors of the Sports, Media &amp; Entertainment industry. Founded by a former professional football player with significant experience from both blue-chip investing realms alongside profound business ties in this sector, Bluestone Equity Partners seeks to deliver sustained value through strategic capital partnerships that focus on high-growth management teams and rights holders. Their recent notable accomplishment includes the closing of their inaugural $300 million growth equity fund targeting these industries globally, exemplified by a significant investment in VideoVerse for content delivery solutions within sports entertainment realms.
 </t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> I'm sorry, but as an AI language model, I don't have access to specific information on the products and services offered by Yamada. However, I can suggest searching online for their official website or contacting them directly for more details. They likely offer a range of products and services related to food, including grocery items, restaurants, and catering. Their website may provide more detailed information about their offerings, pricing, and any promotions or events they are currently running. If you have access to social media, you can also follow Yamada on various platforms to stay updated on their latest news and updates. I hope this helps!
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Bobby Sharma</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>7 employees at their primary location.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>The information provided does not specify if Bluestone Equity Partners operates on a Business-to-Businesses (B2B) model exclusively. However, considering the context of investing in sports media and entertainment businesses alongside partnerships with established entities for capital access within this industry suggests it leans more towards B2B or mixed engagement strategies rather than strictly serving end consumers as a Business-to-Consumers (B2C) firm. Without explicit statements, the safest assumption given its investment focus is that Bluestone Equity Partners operates on at least some level of B2B model within this sector for private equity and growth capital funding purposes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kwik Brain</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kwik Brain, led by CEO Alexis Banc and author Jim Kwik, is a globally recognized brand offering cutting-edge speed reading and memory training programs to busy individuals and organizations seeking efficiency enhancement in learning and life improvement for achieving more with less time. Their services are aimed at transforming the way people interact with their brain performance capabilities while also providing educational content on mental fitness, consciousness awareness, and positive self-talk through podcasts to deepen understanding of one's own cognitive processes.
 </t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Enter the transformative world of accelerated learning with Kwik Brain, offering products and services designed to master new skills quickly, retain vast amounts of information effectively, and significantly boost overall brain power without relying on smart pills or endless brain games—achieving all in just 21 short days. With a strong emphasis on practicality and immediate results, Kwik Brain provides accessibility through various offerings including the highly-praised courses that promise to improve reading speed by up to 300%, alongside comprehensive time management techniques backed by Jim Kwik's expertise as the world’s #1 brain coach. They assure satisfaction with a guarantee on all products, inviting potential customers through their Help Center for further inquiries and specialized offers tailored towards personal improvement such as payment plans or additional programs like 'Kwik Recall Masterclass.'</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Alexis Banc</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2001.0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Kwik Brain is a B2B organization.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kwik Learning</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Established as a renowned authority, Jim Kwik leads global memory and speed reading programs at Kwik Learning for individual clients and Fortune 500 companies worldwide to enhance learning efficiency. As an associate trainer at KwikKianGie School of Business in Jakarta with over 391 LinkedIn connections, he applies practical knowledge there too.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At Kwik Learning, they offer an array of services and products designed to make studying more enjoyable, efficient, and effective for students across all subjects. Leveraging Jim Kwik's top memory and study skills techniques, their platform provides lifel0t access to a comprehensive collection of engaging e-learning courses tailored to master technical and nonfiction material in three easy steps: understanding information better with the use of tools like mind maps or visualization; remembering through chunked learning into bite-sized sections that are easier to memorize, as well as employing techniques such as mnemonics for retention enhancement; recall by applying active review methods and practicing retrieval. Their resources offer a combination of cognitive strategies aimed at improving focus, motivation, and memory consolidation, helping students not only excel academically but also develop skills applicable to real-world tasks outside the classroom environment. They emphasize continuous learning through their programs that promise quick wins for learners while maintaining long-term educational progress. Kwik Student courses mimic advanced techniques used by high achievers in various fields, offering students a streamlined pathway toward academic success and goal achievement with less effort required to study effectively.
+</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$7.4 billion</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>- Jim Kwik</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2001.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Kwik Learning is a B2B and B2C.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kwik Learning</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Kwik Learning is globally recognized as a leader in enhancing memory and reading speed, serving individuals and top-tier corporate clients through their expertise and practical knowledge shared via Kwik Brain Podcast with over 60 million downloads, hosted by Jim Kwik.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Experience accelerated learning with products and services from Kwik Learning, designed to make studying more enjoyable and efficient. Their courses blend Jim Kwik's best memory techniques with proven study methods for improved focus, memorization, and comprehension across subjects, aiming to boost grades and qualifications while enhancing life readiness skills. The 30-day transformative program offers strategies not just academically but in mastering new skills broadly—enabling learners to unleash their inner genius effectively. Kwik Learning also provides discounts for last minute shoppers, making top learning tools accessible and affordable with lifetime access guarantees on the system approach to studying technical materials like math while discovering one's unique learning style through a 3-step process tailored by experts such as Jim Kwik.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$12 million in revenue</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$12 million</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Alexis Banc</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2001.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Kwik Learning is primarily a B2B service. It focuses on business clients like Fortune 500 corporate and educational institutions by offering memory improvement and speed reading training programs. While they do serve individual learners through resources, the core of their services targets organizations for bulk knowledge enhancement within teams or individuals in professional settings as evidenced by articles linked to workshops with a business focus on employee development skills such as studying can be more enjoyable &amp; efficient etc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Born Again Construction LLC</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Born Again Construction, LLC is a contracting firm with objectives to exceed client expectations through dedication and quality work daily, offering both commercial and residential remodeling services while also representing Everest Energy Solutions for environmental opportunities. They maintain connections on LinkedIn and are committed to preserving the planet by giving back in their industry practices.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Welcome to Born Again Construction LLC! As your trusted contractor since 2008, we offer top-notch services in commercial and residential remodels for occupied job sites. Our expertise extends beyond metal buildings as well; our team prides itself on craftsmanship with projects such as barns, storm shelters, excavations, and restorative work at educational institutions. Ready to dream big? We're equipped to design it, plan it, manage it - we do all! With over 30 years of experience under our belt, your project aspirs are within reach through Born Again Construction LLC in Phoenix, AZ and surrounding areas. Don't hesitate – get in touch for exceptional construction services that deliver quality with transparency at every step.
+</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>USD 146,429</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$14 million in annual revenue</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Founder/Owner's Full Name: Not provided in the given information.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>$889</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2008.0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Given the provided information about Born Again Construction LLC and its business activities, it can be categorized under Business to Businesses (B2B). The company operates within construction-related projects such as residential remodels, commercial work, stucco estimating, storm shelters, barns, excavations, metal buildings, and specializes in educational institution renovations. They focus on building trust with quality contracting services for other businesses or property owners who are looking to engage their construction expertise. While they do provide a service that benefits the end user (the clients), their primary operation is delivering construction work which typically involves transactions between companies, developers and Born Again Construction LLC as subcontractors or prime contractors within those industries rather than direct consumer-to-consumer interactions characteristic of B2C.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Veritas Capital Fund Management LLC</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veritas Capital is a technology-focused private equity firm based in New York, with over $40 billion in assets under management. The company primarily invests in technology or technology-enabled solutions for both government and commercial customers worldwide. Veritas Capital's team includes experienced professionals such as Rushin Shah, Alex Chapin, and Hardik Patel. The firm's investments are centered around critical products, services, and software.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veritas Capital Fund Management LLC is an American private-equity firm based in New York, founded in 1992. The firm exclusively invests in companies that provide critical products, services, and software, primarily technology or technology-enabled solutions, to both government and commercial customers worldwide. For over 25 years, Veritas Capital has focused on investing in companies that offer essential solutions to a wide range of industries.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Veritas Capital Fund Management LLC</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veritas Capital is a technology-focused private equity firm with over $40 billion in assets under management. They invest in companies at the intersection of technology and government. The firm works with portfolio companies as board members to guide strategy, and their team includes partners like Alex Chapin, Hardik Patel, Alexander K., and Brendan Dillon. The company is based in New York. (Company Overview)
+Veritas Capital offers private equity investment services, focusing on technology-centric companies. (Products &amp; Services)
+Not Found (Revenue)
+Not Found (Founder or CEO)
+Not Found (Employee Count)
+Not Found (Year Founded)
+B2B (Business Type)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veritas Capital is a New York-based private equity firm founded in 1992. They specialize in investing in companies that provide critical products, services, and software, primarily technology-enabled solutions, to government and commercial customers worldwide. Over the past 25 years, Veritas has exclusively focused on this niche, with their eighth flagship fund closing in 2022, bringing their total assets under management to approximately $45 billion. (Company Overview)
+Veritas Capital offers investment services to companies providing technology-centric products and services to both government and commercial customers. (Products &amp; Services)
+Not Found (Revenue)
+Veritas Capital was founded in 1992. (Year Founded)
+Not Found (Founder or CEO)
+Not Found (Employee Count)
+B2B (Business Type)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Born Again Construction LLC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Born Again Construction LLC</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1. 🏢 Company Overview  
+"Born Again Construction LLC is a general contractor specializing in commercial and residential remodels. The company handles occupied and operational job sites and also plans, manages, and builds multi-property projects. It serves both commercial and residential clients."  
+2. 🛠️ Products &amp; Services  
+"Provides general contracting services for commercial and residential remodels, including planning, managing, and building multi-property projects."  
+3. 💰 Revenue  
+Not Found  
+4. 👤 Founder or CEO  
+Not Found  
+5. 🧍 Employee Count  
+Not Found  
+6. 🗓️ Year Founded  
+Not Found  
+7. 🔁 Business Type  
+"B2B, B2C" (serves both commercial and residential clients)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1. 🏢 Company Overview  
+Born Again Construction LLC is a construction company specializing in commercial and residential remodels, metal buildings, excavations, barns, and storm shelters. They serve clients in East Texas and Glendale, AZ, with expertise in occupied and operational job sites, as well as educational institution remodeling.  
+2. 🛠️ Products &amp; Services  
+Provides construction and remodeling services, including commercial and residential projects, metal buildings, excavations, barns, storm shelters, and design-build solutions.  
+3. 💰 Revenue  
+Not Found  
+4. 👤 Founder or CEO  
+Not Found  
+5. 🧍 Employee Count  
+Not Found  
+6. 🗓️ Year Founded  
+2008  
+7. 🔁 Business Type  
+B2B, B2C</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$146.43K</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>$1M-$5M</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>$234.92K</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>6-10</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>1. 🏢 Company Overview  
+"Born Again Construction LLC is a construction company specializing in commercial and residential remodels, metal buildings, excavations, barns, and storm shelters. They serve clients in East Texas and Arizona, offering design, planning, and project management services."
+2. 🛠️ Products &amp; Services  
+"Provides construction and remodeling services for both commercial and residential projects, including metal buildings, storm shelters, and excavations."
+3. 💰 Revenue  
+Not Found  
+4. 👤 Founder or CEO  
+Not Found  
+5. 🧍 Employee Count  
+Not Found  
+6. 🗓️ Year Founded  
+2008  
+7. 🔁 Business Type  
+B2B, B2C</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Born Again Construction LLC</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Born Again Construction LLC is a general contracting company specializing in commercial and residential remodels, including occupied job sites. They emphasize exceeding client expectations and have experience in remodeling educational institutions. The company operates in locations like Fountain Hills and Montclair, with a focus on quality and faith-driven values.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Born Again Construction LLC offers a range of construction and remodeling services for both commercial and residential projects. Their expertise includes metal buildings, excavations, barns, storm shelters, and remodels, with a focus on occupied and operational job sites. They provide planning, management, and building services, including design work for expansions or new spaces. The company has experience in remodeling educational institutions and emphasizes quality craftsmanship. Operating since 2008, they serve areas like East Texas and Glendale, AZ, handling projects such as commercial permits and home improvements. Their mission is to deliver high-quality contracting work with attention to detail.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>USD 146,429</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>USD 146,429</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>234921</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Not Found.</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>B2C</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Veritas Capital Fund Management LLC</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Veritas Capital is a longstanding technology investment firm with over $40 billion in assets under management. It focuses on companies in technology sectors and engages in private equity investments, due diligence, and portfolio management. Key team members include Rushin Shah (Managing Director, Credit) and Jeffrey W. (Partner). Location: New York.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Veritas Capital Fund Management LLC is a New York-based private equity firm founded in 1992. It invests in companies that provide critical products, services, and software, primarily technology or technology-enabled solutions, to government and commercial customers worldwide. The firm focuses on sectors such as defense, aerospace, and other mission-critical industries. With over 25 years of experience, Veritas Capital specializes in supporting businesses that deliver essential solutions to government and commercial clients, emphasizing innovation and technology-driven services. Its investment strategy centers on companies that offer high-value, technology-based products and services in key industries.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Veritas Capital Fund Management LLC</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Veritas Capital is a technology-focused investment firm with over $40 billion in assets under management. It has a team of professionals, including partners and managing directors, who oversee private equity investments and work with portfolio companies on strategy. Notable team members include Rushin Shah and Varun Bhardwaj.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Veritas Capital Fund Management LLC is a New York-based private equity firm founded in 1992. It specializes in investing in companies that provide critical products, services, and software, primarily technology or technology-enabled solutions, to government and commercial customers worldwide. The firm focuses on sectors such as defense, aerospace, and government technology. With over 25 years of experience, Veritas Capital exclusively targets businesses delivering mission-critical solutions, emphasizing innovation in these areas. Its investments support companies that serve both public and private sector clients globally. The firm’s strategy centers on acquiring and growing businesses that offer essential technological and service-based solutions.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>